<commit_message>
Land-use variables with Brazilian specific data
</commit_message>
<xml_diff>
--- a/InputData/land/AOCoLUPpUA/Annual Ongoing Cost of Land Use Pol per Unit Area.xlsx
+++ b/InputData/land/AOCoLUPpUA/Annual Ongoing Cost of Land Use Pol per Unit Area.xlsx
@@ -1,45 +1,35 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25028"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28129"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mmahajan\Documents\eps-us\InputData\land\AOCoLUPpUA\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\anima\Box\Brazil calibration\land\AOCoLUPpUA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF94B7C1-28EB-4AAB-A6C5-9A13131631C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66CCEBD2-2117-4ED2-94A9-397D3295292C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
-    <sheet name="AOCoLUPpUA" sheetId="3" r:id="rId2"/>
+    <sheet name="Data" sheetId="4" r:id="rId2"/>
+    <sheet name="Conversions" sheetId="5" r:id="rId3"/>
+    <sheet name="AOCoLUPpUA" sheetId="3" r:id="rId4"/>
   </sheets>
   <externalReferences>
-    <externalReference r:id="rId3"/>
+    <externalReference r:id="rId5"/>
   </externalReferences>
   <definedNames>
     <definedName name="C_to_CO2">'[1]Conversion Factors'!$A$4</definedName>
   </definedNames>
-  <calcPr calcId="191029" iterate="1" iterateDelta="1.0000000000000001E-5"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
+  <calcPr calcId="181029"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="86">
   <si>
     <t>AOCoLUPpUA Annual Ongoing Cost of Land Use Policies per Unit Area</t>
   </si>
@@ -71,9 +61,6 @@
     <t>annual maintenance cost ($ / acre)</t>
   </si>
   <si>
-    <t>None</t>
-  </si>
-  <si>
     <t xml:space="preserve">Based on consultation with the organization American Forests, </t>
   </si>
   <si>
@@ -84,13 +71,233 @@
   </si>
   <si>
     <t>to track these in the US model.</t>
+  </si>
+  <si>
+    <t>de Souza Cunha et. al used  2.5 R$/US$ for all of their computations</t>
+  </si>
+  <si>
+    <t>Unit Conversions</t>
+  </si>
+  <si>
+    <t>Study: "Minimum costs to conserve 80% of the Brazilian Amazon"</t>
+  </si>
+  <si>
+    <t>da Silva, J. M. C., Barbosa, L. C. F., Topf, J., Vieira, I. C. G., &amp; Scarano, F. R. (2022). Minimum costs to conserve 80% of the Brazilian Amazon. Perspectives in Ecology and Conservation, 20(3), 216-222.</t>
+  </si>
+  <si>
+    <t>doi.org/10.1016/j.pecon.2022.03.007</t>
+  </si>
+  <si>
+    <t>Study: "The implementation costs of forest conservation policies in Brazil"</t>
+  </si>
+  <si>
+    <t>de Souza Cunha, F. A. F., Börner, J., Wunder, S., Cosenza, C. A. N., &amp; Lucena, A. F. (2016). The implementation costs of forest conservation policies in Brazil. Ecological economics, 130, 209-220.</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1016/j.ecolecon.2016.07.007</t>
+  </si>
+  <si>
+    <t>Report: "Defining the Real Cost of Restoring Forests"</t>
+  </si>
+  <si>
+    <t>Trillion Trees</t>
+  </si>
+  <si>
+    <t>https://trilliontrees.org/wp-content/uploads/2022/08/Trillion-Trees_Defining-the-real-cost-of-restoring-forests.pdf</t>
+  </si>
+  <si>
+    <t>Study: "A landscape approach for cost-effective large-scale forestrestoration"</t>
+  </si>
+  <si>
+    <t>Molin, P. G., Chazdon, R., Frosini de Barros Ferraz, S., &amp; Brancalion, P. H. (2018). A landscape approach for cost‐effective large‐scale forest restoration. Journal of Applied Ecology, 55(6), 2767-2778.</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1111/1365-2664.13263</t>
+  </si>
+  <si>
+    <t>Report: "Economics of
+Peatlands Conservation, Restoration and Sustainable Management"</t>
+  </si>
+  <si>
+    <t>UNEP</t>
+  </si>
+  <si>
+    <t>https://www.uncclearn.org/wp-content/uploads/library/PeatCRSM.pdf#:~:text=Investing%20in%20cost%2Deffective%20tropical%20peatland%20conservation%20and,and%20US$11.7%20billion%20more%20for%20restoration%20(</t>
+  </si>
+  <si>
+    <t>Study: "Caracterização de Organossolos, auxílio à sua classificação"</t>
+  </si>
+  <si>
+    <t>Valladares, G. S. (2003). Caracterização de Organossolos, auxílio à sua classificação. Seropédica: Universidade Federal Rural do Rio de Janeiro.</t>
+  </si>
+  <si>
+    <t>Forests Set Aside</t>
+  </si>
+  <si>
+    <t>Avoided Deforestation</t>
+  </si>
+  <si>
+    <t>Improved Forest Management</t>
+  </si>
+  <si>
+    <t>Forest Restoration</t>
+  </si>
+  <si>
+    <t>Reforestation</t>
+  </si>
+  <si>
+    <t>Peatland Restoration</t>
+  </si>
+  <si>
+    <t>Minimum costs to conserve 80% of the Brazilian Amazon</t>
+  </si>
+  <si>
+    <t>The implementation costs of forest conservation policies in Brazil</t>
+  </si>
+  <si>
+    <t>2005-2013</t>
+  </si>
+  <si>
+    <t>Defining the Real Cost of Restoring Forests</t>
+  </si>
+  <si>
+    <t>Economics of Peatlands Conservation, Restoration and Sustainable Management</t>
+  </si>
+  <si>
+    <t>Area</t>
+  </si>
+  <si>
+    <t>Annual Maintenance Cost</t>
+  </si>
+  <si>
+    <t>Priority Conservation Areas</t>
+  </si>
+  <si>
+    <t>Price of management per hectare</t>
+  </si>
+  <si>
+    <t>Natural Regeneration</t>
+  </si>
+  <si>
+    <t>Fencing and Planting (Combined)</t>
+  </si>
+  <si>
+    <t>Annual Restoration Cost</t>
+  </si>
+  <si>
+    <t>Price</t>
+  </si>
+  <si>
+    <t>Price per hectare</t>
+  </si>
+  <si>
+    <t>Annual Management Cost</t>
+  </si>
+  <si>
+    <t>Note: Area in (km^2) and Cost in mil $USD, annual cost is average of mil $USD 305.6-488.9, adds initial investment of 550.1–880.0 mil $USD required</t>
+  </si>
+  <si>
+    <t>Note: Area in Units of km^2 and Price in $USD/ha</t>
+  </si>
+  <si>
+    <t>Note: Units of $USD/ha, mean of given range (385–1153)</t>
+  </si>
+  <si>
+    <t>Note: Cost denoted in mil $USD</t>
+  </si>
+  <si>
+    <t>A landscape approach for cost-effective large-scale forestrestoration</t>
+  </si>
+  <si>
+    <t>Cost total</t>
+  </si>
+  <si>
+    <t>Plantations &amp; Pasturelands</t>
+  </si>
+  <si>
+    <t>Caracterização de Organossolos, auxílio à sua classificação</t>
+  </si>
+  <si>
+    <t>$USD per hectare</t>
+  </si>
+  <si>
+    <t>Hectares of Brazilian Peatlands</t>
+  </si>
+  <si>
+    <t>Note: Cost in $USD bil and is an average of the given range (1.7-2.8), Area in hectares, adds initial investment 1.0-1.6 bil $USD would be required</t>
+  </si>
+  <si>
+    <t>Improved Forest Management &amp; Forests Set Aside</t>
+  </si>
+  <si>
+    <t>Improved Forest Management &amp; Avoid Deforestation</t>
+  </si>
+  <si>
+    <t>Forest Restoration &amp; Reforestation</t>
+  </si>
+  <si>
+    <t>Note: Denoted in $</t>
+  </si>
+  <si>
+    <t>Forest restoration &amp; reforestation data for Atlantic forest area</t>
+  </si>
+  <si>
+    <t>Initial Unit</t>
+  </si>
+  <si>
+    <t>$USD2012/Acre</t>
+  </si>
+  <si>
+    <t>Given 2 conflicting sources for forest restoration &amp; reforestation, Molin defaulted to</t>
+  </si>
+  <si>
+    <t>acre/km^2</t>
+  </si>
+  <si>
+    <t>acre/ha</t>
+  </si>
+  <si>
+    <t>Conversions via housing.com/calculators/</t>
+  </si>
+  <si>
+    <t>$USD 2012/2022</t>
+  </si>
+  <si>
+    <t>Conversions via in2013dollars.com/us/inflation/</t>
+  </si>
+  <si>
+    <t>$2022USD/km^2</t>
+  </si>
+  <si>
+    <t>$2018USD/ha</t>
+  </si>
+  <si>
+    <t>$USD 2012/2018</t>
+  </si>
+  <si>
+    <t>$2020USD/ha</t>
+  </si>
+  <si>
+    <t>$USD 2012/2020</t>
+  </si>
+  <si>
+    <t>$2013USD/ha</t>
+  </si>
+  <si>
+    <t>Forest management figure via de Souza Cunha</t>
+  </si>
+  <si>
+    <t>$USD 2012/2013</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
+  </numFmts>
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -129,13 +336,34 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF222222"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="5">
@@ -183,7 +411,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="7">
+  <cellStyleXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" applyNumberFormat="0" applyFont="0" applyProtection="0">
       <alignment wrapText="1"/>
@@ -201,19 +429,37 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyProtection="0">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="7"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="7">
+  <cellStyles count="8">
     <cellStyle name="Body: normal cell" xfId="1" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
     <cellStyle name="Font: Calibri, 9pt regular" xfId="2" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
     <cellStyle name="Footnotes: top row" xfId="3" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
     <cellStyle name="Header: bottom row" xfId="4" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Parent row" xfId="5" xr:uid="{00000000-0005-0000-0000-000006000000}"/>
     <cellStyle name="Table title" xfId="6" xr:uid="{00000000-0005-0000-0000-000007000000}"/>
@@ -232,7 +478,7 @@
 </file>
 
 <file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
       <sheetName val="About"/>
@@ -289,9 +535,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -329,9 +575,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -364,26 +610,9 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -416,26 +645,9 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -609,63 +821,249 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B21"/>
+  <dimension ref="A1:E53"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+    <sheetView topLeftCell="A25" zoomScale="61" zoomScaleNormal="10" workbookViewId="0">
+      <selection activeCell="B54" sqref="B54"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="15" customWidth="1"/>
+    <col min="2" max="2" width="45.81640625" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="14.45" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="6" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="29" x14ac:dyDescent="0.35">
+      <c r="B4" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="58" x14ac:dyDescent="0.35">
+      <c r="B5" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B6" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B7" s="3"/>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B8" s="8" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" ht="29" x14ac:dyDescent="0.35">
+      <c r="B9" s="3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" ht="58" x14ac:dyDescent="0.35">
+      <c r="B10" s="4" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B11" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B13" s="6" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B14" s="3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B15" s="3">
+        <v>2022</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B16" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B17" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B19" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" ht="58" x14ac:dyDescent="0.35">
+      <c r="B20" s="3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B21" s="5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B22" s="5"/>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B23" s="6" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="B24" s="3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A25" s="1"/>
+      <c r="B25">
+        <v>2021</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B26" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B27" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B29" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="B30" s="3" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A36" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A37" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="14.45" x14ac:dyDescent="0.35">
-      <c r="A5" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A38" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" s="4" t="s">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A39" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" s="4" t="s">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A40" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" s="4" t="s">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A42" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="10" spans="1:2" ht="14.45" x14ac:dyDescent="0.35"/>
-    <row r="11" spans="1:2" ht="14.45" x14ac:dyDescent="0.35"/>
-    <row r="13" spans="1:2" ht="14.45" x14ac:dyDescent="0.35"/>
-    <row r="14" spans="1:2" ht="14.45" x14ac:dyDescent="0.35"/>
-    <row r="15" spans="1:2" ht="14.45" x14ac:dyDescent="0.35"/>
-    <row r="16" spans="1:2" ht="14.45" x14ac:dyDescent="0.35"/>
-    <row r="17" spans="1:1" ht="14.45" x14ac:dyDescent="0.35"/>
-    <row r="18" spans="1:1" ht="14.45" x14ac:dyDescent="0.35"/>
-    <row r="19" spans="1:1" ht="14.45" x14ac:dyDescent="0.35"/>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A21" s="1"/>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A44" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A45" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A46" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="A48" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B48">
+        <v>247.10538149999999</v>
+      </c>
+      <c r="C48" t="s">
+        <v>73</v>
+      </c>
+      <c r="E48" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="49" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B49">
+        <v>2.4710538149999999</v>
+      </c>
+      <c r="C49" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="50" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B50" s="10">
+        <v>0.78</v>
+      </c>
+      <c r="C50" t="s">
+        <v>76</v>
+      </c>
+      <c r="E50" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="51" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B51" s="10">
+        <v>0.91</v>
+      </c>
+      <c r="C51" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="52" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B52" s="10">
+        <v>0.89</v>
+      </c>
+      <c r="C52" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="53" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B53" s="10">
+        <v>0.99</v>
+      </c>
+      <c r="C53" t="s">
+        <v>85</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -673,6 +1071,349 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{12F9DBDF-7604-4AD0-BB5C-D94708805B33}">
+  <dimension ref="A2:W13"/>
+  <sheetViews>
+    <sheetView topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="G10" sqref="G10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="42.81640625" customWidth="1"/>
+    <col min="7" max="7" width="31.90625" customWidth="1"/>
+    <col min="10" max="10" width="28.81640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="16.1796875" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="23.81640625" customWidth="1"/>
+    <col min="22" max="22" width="37.7265625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A2" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="G2" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="J2" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="M2" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q2" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="V2" s="6" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="3" spans="1:23" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A3" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="B3">
+        <v>2022</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="H3" t="s">
+        <v>41</v>
+      </c>
+      <c r="J3" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="K3" t="s">
+        <v>41</v>
+      </c>
+      <c r="M3" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q3" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="V3" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="W3">
+        <v>2020</v>
+      </c>
+    </row>
+    <row r="4" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A4" s="3"/>
+      <c r="B4" t="s">
+        <v>44</v>
+      </c>
+      <c r="C4" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="5" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A5" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="B5" s="7">
+        <v>780416</v>
+      </c>
+      <c r="C5">
+        <v>397.25</v>
+      </c>
+      <c r="G5" t="s">
+        <v>44</v>
+      </c>
+      <c r="H5" s="7">
+        <v>36780</v>
+      </c>
+      <c r="J5" t="s">
+        <v>47</v>
+      </c>
+      <c r="K5">
+        <v>615.5</v>
+      </c>
+      <c r="N5" t="s">
+        <v>48</v>
+      </c>
+      <c r="R5" t="s">
+        <v>49</v>
+      </c>
+      <c r="V5" t="s">
+        <v>50</v>
+      </c>
+      <c r="W5">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="6" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A6" s="3"/>
+      <c r="G6" t="s">
+        <v>51</v>
+      </c>
+      <c r="H6">
+        <v>462</v>
+      </c>
+      <c r="M6" t="s">
+        <v>52</v>
+      </c>
+      <c r="N6">
+        <v>1250</v>
+      </c>
+      <c r="Q6" t="s">
+        <v>52</v>
+      </c>
+      <c r="R6">
+        <v>3750</v>
+      </c>
+      <c r="V6" t="s">
+        <v>53</v>
+      </c>
+      <c r="W6">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="7" spans="1:23" ht="58" x14ac:dyDescent="0.35">
+      <c r="A7" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="G7" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="J7" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="M7" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="Q7" s="3" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="8" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="V8" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="9" spans="1:23" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="A9" s="3"/>
+      <c r="G9" s="3"/>
+      <c r="J9" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="M9" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="N9">
+        <v>2018</v>
+      </c>
+      <c r="Q9" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="R9">
+        <v>2018</v>
+      </c>
+    </row>
+    <row r="10" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="J10" t="s">
+        <v>59</v>
+      </c>
+      <c r="K10">
+        <v>2.25</v>
+      </c>
+      <c r="N10" t="s">
+        <v>48</v>
+      </c>
+      <c r="R10" t="s">
+        <v>60</v>
+      </c>
+      <c r="V10" t="s">
+        <v>61</v>
+      </c>
+      <c r="W10">
+        <v>2003</v>
+      </c>
+    </row>
+    <row r="11" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="J11" t="s">
+        <v>44</v>
+      </c>
+      <c r="K11">
+        <v>350</v>
+      </c>
+      <c r="M11" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="N11">
+        <v>500</v>
+      </c>
+      <c r="Q11" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="R11">
+        <v>3750</v>
+      </c>
+      <c r="V11" t="s">
+        <v>63</v>
+      </c>
+      <c r="W11">
+        <v>611883</v>
+      </c>
+    </row>
+    <row r="13" spans="1:23" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="J13" s="3" t="s">
+        <v>64</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9E425677-DCDD-4D12-AE6E-5D89F2CFDCBC}">
+  <dimension ref="A1:G7"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="27" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.7265625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.453125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.81640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="B1" s="11" t="s">
+        <v>70</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="D1" s="11"/>
+      <c r="E1" s="11"/>
+      <c r="F1" s="11"/>
+      <c r="G1" s="11"/>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A2" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" t="s">
+        <v>78</v>
+      </c>
+      <c r="C2" s="10">
+        <f>Data!C5*About!B50*1000000/(About!B48*Data!B5)</f>
+        <v>1.6067567766372453</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A3" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" t="s">
+        <v>79</v>
+      </c>
+      <c r="C3" s="10">
+        <f>Data!R11*About!B51/About!B49</f>
+        <v>1380.9897539604981</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A4" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" t="s">
+        <v>83</v>
+      </c>
+      <c r="C4" s="10">
+        <f>Data!K5*About!B53/About!B49</f>
+        <v>246.59317263796623</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A5" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" t="s">
+        <v>83</v>
+      </c>
+      <c r="C5" s="10">
+        <f>Data!H6*About!B53/About!B49</f>
+        <v>185.09511902313631</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A6" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" t="s">
+        <v>81</v>
+      </c>
+      <c r="C6" s="10">
+        <f>1000000*Data!W5*About!B52/(Data!W11*About!B48)</f>
+        <v>1.2361145271989211</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A7" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="B7" t="s">
+        <v>79</v>
+      </c>
+      <c r="C7" s="10">
+        <f>Data!N11*About!B51/About!B49</f>
+        <v>184.13196719473308</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr>
     <tabColor theme="3"/>
@@ -680,12 +1421,12 @@
   <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A36" sqref="A36"/>
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="31.140625" customWidth="1"/>
+    <col min="1" max="1" width="31.1796875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
@@ -697,48 +1438,54 @@
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="2">
-        <v>0</v>
+      <c r="B2" s="12">
+        <f>Conversions!C2</f>
+        <v>1.6067567766372453</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="2">
-        <v>0</v>
+      <c r="B3" s="12">
+        <f>Conversions!C3</f>
+        <v>1380.9897539604981</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="3">
-        <v>0</v>
+      <c r="B4" s="12">
+        <f>Conversions!C4</f>
+        <v>246.59317263796623</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="2">
-        <v>0</v>
+      <c r="B5" s="12">
+        <f>Conversions!C5</f>
+        <v>185.09511902313631</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="2">
-        <v>0</v>
+      <c r="B6" s="12">
+        <f>Conversions!C6</f>
+        <v>1.2361145271989211</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B7" s="2">
-        <v>0</v>
+      <c r="B7" s="12">
+        <f>Conversions!C7</f>
+        <v>184.13196719473308</v>
       </c>
     </row>
   </sheetData>

</xml_diff>